<commit_message>
Update DateBase/orders/Fresh bloom Flowers_2025-9-25.xlsx
</commit_message>
<xml_diff>
--- a/DateBase/orders/Fresh bloom Flowers_2025-9-25.xlsx
+++ b/DateBase/orders/Fresh bloom Flowers_2025-9-25.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -497,9 +497,60 @@
         <v>46_拉丝橙_Spider orange_Gerbera L._20stems</v>
       </c>
     </row>
+    <row r="12">
+      <c r="C12" t="str">
+        <v>42_拉丝黄_Spider Yellow_Gerbera L._20stems</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="C13" t="str">
+        <v>546_绿宝石_undefined_undefined_1bunch</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="C14" t="str">
+        <v>49_亚丁_Pasta Rosata_Gerbera L._10stems</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="C15" t="str">
+        <v>84_堪培拉_undefined_Gerbera L._10stems</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="C16" t="str">
+        <v>393_天堂鸟_strelitzia reginae_undefined_1bunch</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="C17" t="str">
+        <v>516_火焰兰_Crocosmia_undefined_1bunch</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="C18" t="str">
+        <v>479_绿灵草_lepidium_undefined_1bunch</v>
+      </c>
+    </row>
+    <row r="19" xml:space="preserve">
+      <c r="C19" t="str" xml:space="preserve">
+        <v xml:space="preserve">386_菟葵绿粉 
+green_undefined_undefined_1bunch</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="C20" t="str">
+        <v>449_柔丽思 绿_undefined_undefined_1bunch</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="C21" t="str">
+        <v>450_柔丽思 黄_undefined_undefined_1bunch</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L11"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L21"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -557,7 +608,7 @@
         <v>0.00</v>
       </c>
       <c r="G2" t="str">
-        <v>052000000000</v>
+        <v>0520000000000000000000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>